<commit_message>
Pushing company Add and Company Delete scripts
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Tc01</t>
   </si>
@@ -73,6 +73,30 @@
   </si>
   <si>
     <t>Gaurav.bh@gmail.com</t>
+  </si>
+  <si>
+    <t>Tc03</t>
+  </si>
+  <si>
+    <t>PkiCompanyAdd</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>GbTestCompany</t>
+  </si>
+  <si>
+    <t>CompanyEmail</t>
+  </si>
+  <si>
+    <t>AuthStartDate</t>
+  </si>
+  <si>
+    <t>6/14/2017</t>
+  </si>
+  <si>
+    <t>Gaurav.bharti@trivium.com</t>
   </si>
 </sst>
 </file>
@@ -125,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -146,6 +170,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,18 +452,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
@@ -528,11 +553,41 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1"/>
     <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>